<commit_message>
spider returned right value
</commit_message>
<xml_diff>
--- a/resources/documents/faculty_info.xlsx
+++ b/resources/documents/faculty_info.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hackroid/Code/Faculty-Reservation/resources/documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E00AB5-DB81-734B-BE0C-1C07343F0402}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="工作表1" sheetId="1" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -487,17 +496,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -505,54 +525,360 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.43"/>
-    <col customWidth="1" min="3" max="3" width="65.57"/>
-    <col customWidth="1" min="4" max="4" width="29.57"/>
-    <col customWidth="1" min="6" max="6" width="58.14"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="58.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -583,18 +909,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -605,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -616,7 +942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -627,7 +953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -638,7 +964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -649,7 +975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -671,7 +997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -682,7 +1008,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -693,7 +1019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -704,7 +1030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -715,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -726,7 +1052,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -737,7 +1063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -748,7 +1074,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -759,7 +1085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -770,7 +1096,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -781,7 +1107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -792,7 +1118,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -803,7 +1129,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -814,7 +1140,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -825,7 +1151,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -836,7 +1162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -847,7 +1173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -858,7 +1184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
@@ -869,7 +1195,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -880,7 +1206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -891,7 +1217,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -902,7 +1228,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
@@ -913,7 +1239,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -924,7 +1250,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -935,7 +1261,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -946,7 +1272,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
@@ -957,7 +1283,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>80</v>
       </c>
@@ -968,7 +1294,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>80</v>
       </c>
@@ -979,7 +1305,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -990,7 +1316,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>80</v>
       </c>
@@ -1001,7 +1327,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1012,7 +1338,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
@@ -1023,7 +1349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
@@ -1034,7 +1360,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
@@ -1045,7 +1371,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>91</v>
       </c>
@@ -1056,7 +1382,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>91</v>
       </c>
@@ -1067,7 +1393,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
@@ -1078,7 +1404,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>102</v>
       </c>
@@ -1089,7 +1415,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>102</v>
       </c>
@@ -1100,7 +1426,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
@@ -1111,7 +1437,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>102</v>
       </c>
@@ -1122,7 +1448,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
@@ -1133,7 +1459,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
@@ -1144,7 +1470,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -1155,7 +1481,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
@@ -1166,7 +1492,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>113</v>
       </c>
@@ -1177,7 +1503,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
@@ -1188,7 +1514,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>124</v>
       </c>
@@ -1199,7 +1525,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
@@ -1210,7 +1536,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>124</v>
       </c>
@@ -1221,7 +1547,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -1232,7 +1558,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>135</v>
       </c>
@@ -1243,7 +1569,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>135</v>
       </c>
@@ -1254,7 +1580,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>135</v>
       </c>
@@ -1265,7 +1591,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>135</v>
       </c>
@@ -1276,7 +1602,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
@@ -1287,7 +1613,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>146</v>
       </c>
@@ -1298,7 +1624,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>146</v>
       </c>
@@ -1309,7 +1635,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>146</v>
       </c>
@@ -1320,7 +1646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>146</v>
       </c>
@@ -1331,7 +1657,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>146</v>
       </c>
@@ -1344,77 +1670,77 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
-    <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" ref="C5"/>
-    <hyperlink r:id="rId5" ref="C6"/>
-    <hyperlink r:id="rId6" ref="C7"/>
-    <hyperlink r:id="rId7" ref="C8"/>
-    <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C10"/>
-    <hyperlink r:id="rId10" ref="C11"/>
-    <hyperlink r:id="rId11" ref="C12"/>
-    <hyperlink r:id="rId12" ref="C13"/>
-    <hyperlink r:id="rId13" ref="C14"/>
-    <hyperlink r:id="rId14" ref="C15"/>
-    <hyperlink r:id="rId15" ref="C16"/>
-    <hyperlink r:id="rId16" ref="C17"/>
-    <hyperlink r:id="rId17" ref="C18"/>
-    <hyperlink r:id="rId18" ref="C19"/>
-    <hyperlink r:id="rId19" ref="C20"/>
-    <hyperlink r:id="rId20" ref="C21"/>
-    <hyperlink r:id="rId21" ref="C22"/>
-    <hyperlink r:id="rId22" ref="C23"/>
-    <hyperlink r:id="rId23" ref="C24"/>
-    <hyperlink r:id="rId24" ref="C25"/>
-    <hyperlink r:id="rId25" ref="C26"/>
-    <hyperlink r:id="rId26" ref="C27"/>
-    <hyperlink r:id="rId27" ref="C28"/>
-    <hyperlink r:id="rId28" ref="C29"/>
-    <hyperlink r:id="rId29" ref="C30"/>
-    <hyperlink r:id="rId30" ref="C31"/>
-    <hyperlink r:id="rId31" ref="C32"/>
-    <hyperlink r:id="rId32" ref="C33"/>
-    <hyperlink r:id="rId33" ref="C34"/>
-    <hyperlink r:id="rId34" ref="C35"/>
-    <hyperlink r:id="rId35" ref="C36"/>
-    <hyperlink r:id="rId36" ref="C37"/>
-    <hyperlink r:id="rId37" ref="C38"/>
-    <hyperlink r:id="rId38" ref="C39"/>
-    <hyperlink r:id="rId39" ref="C40"/>
-    <hyperlink r:id="rId40" ref="C41"/>
-    <hyperlink r:id="rId41" ref="C42"/>
-    <hyperlink r:id="rId42" ref="C43"/>
-    <hyperlink r:id="rId43" ref="C44"/>
-    <hyperlink r:id="rId44" ref="C45"/>
-    <hyperlink r:id="rId45" ref="C46"/>
-    <hyperlink r:id="rId46" ref="C47"/>
-    <hyperlink r:id="rId47" ref="C48"/>
-    <hyperlink r:id="rId48" ref="C49"/>
-    <hyperlink r:id="rId49" ref="C50"/>
-    <hyperlink r:id="rId50" ref="C51"/>
-    <hyperlink r:id="rId51" ref="C52"/>
-    <hyperlink r:id="rId52" ref="C53"/>
-    <hyperlink r:id="rId53" ref="C54"/>
-    <hyperlink r:id="rId54" ref="C55"/>
-    <hyperlink r:id="rId55" ref="C56"/>
-    <hyperlink r:id="rId56" ref="C57"/>
-    <hyperlink r:id="rId57" ref="C58"/>
-    <hyperlink r:id="rId58" ref="C59"/>
-    <hyperlink r:id="rId59" ref="C60"/>
-    <hyperlink r:id="rId60" ref="C61"/>
-    <hyperlink r:id="rId61" ref="C62"/>
-    <hyperlink r:id="rId62" ref="C63"/>
-    <hyperlink r:id="rId63" ref="C64"/>
-    <hyperlink r:id="rId64" ref="C65"/>
-    <hyperlink r:id="rId65" ref="C66"/>
-    <hyperlink r:id="rId66" ref="C67"/>
-    <hyperlink r:id="rId67" ref="C68"/>
-    <hyperlink r:id="rId68" ref="C69"/>
-    <hyperlink r:id="rId69" ref="C70"/>
-    <hyperlink r:id="rId70" ref="C71"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>